<commit_message>
Model works (1829.4 val obtained)
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maris\Documents\GitHub\AE4316P Human Machine Systems\AE4441-16-Assignment-code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dani\AE4441-16-Assignment-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF53E22-CA1A-44A7-A3E9-868E9208B38F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F374604F-AEBB-44B6-A6AA-6113E2A9835B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="754" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="754" firstSheet="4" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,9 @@
     <sheet name="gS" sheetId="17" r:id="rId17"/>
     <sheet name="fj" sheetId="18" r:id="rId18"/>
     <sheet name="fS" sheetId="19" r:id="rId19"/>
-    <sheet name="Sheet12" sheetId="20" r:id="rId20"/>
+    <sheet name="thetai" sheetId="20" r:id="rId20"/>
+    <sheet name="deltai" sheetId="21" r:id="rId21"/>
+    <sheet name="taui" sheetId="22" r:id="rId22"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="28">
   <si>
     <t># aj[j], dj[j]                   : expected arrival/departure time of flight j</t>
   </si>
@@ -466,24 +468,24 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
@@ -501,9 +503,9 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -520,7 +522,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -540,7 +542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -560,7 +562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -580,7 +582,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -600,7 +602,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -620,7 +622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -640,7 +642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -660,7 +662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -680,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -713,9 +715,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -732,7 +734,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -752,7 +754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -772,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -792,7 +794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -812,7 +814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -832,7 +834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -852,7 +854,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -872,7 +874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -892,7 +894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -925,9 +927,9 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -944,7 +946,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -964,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -984,7 +986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1004,7 +1006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1024,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1064,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1084,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1104,7 +1106,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1135,9 +1137,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1.2E-2</v>
       </c>
@@ -1155,9 +1157,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1.2E-2</v>
       </c>
@@ -1175,9 +1177,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1.2E-2</v>
       </c>
@@ -1195,9 +1197,9 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1214,7 +1216,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1244,9 +1246,9 @@
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1263,7 +1265,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1293,9 +1295,9 @@
       <selection activeCell="E1" sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1312,7 +1314,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1338,13 +1340,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B4D2BB-7103-4AF3-8248-7F7E94B31278}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1361,7 +1363,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1391,9 +1393,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1410,7 +1412,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>5</v>
       </c>
@@ -1435,12 +1437,118 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CA11B1A-95B9-4BE2-9E32-8EB9D804D9FD}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1.6</v>
+      </c>
+      <c r="C2">
+        <v>1.2</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E21B2EE-AB9E-4139-9D86-9BEEF0A3BA79}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2CDBA43-C340-4F39-8F7C-56EA4E127EAB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1453,9 +1561,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1472,7 +1580,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>120</v>
       </c>
@@ -1502,9 +1610,9 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -1521,7 +1629,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1541,7 +1649,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1561,7 +1669,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1581,7 +1689,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1601,7 +1709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1621,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1641,7 +1749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1661,7 +1769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1681,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1715,9 +1823,9 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>18</v>
       </c>
@@ -1734,7 +1842,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -1754,7 +1862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1774,7 +1882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1794,7 +1902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1814,7 +1922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1834,7 +1942,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1854,7 +1962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1874,7 +1982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1894,7 +2002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1927,9 +2035,9 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -1949,7 +2057,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +2077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1989,7 +2097,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -2009,7 +2117,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2029,7 +2137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2049,7 +2157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2069,7 +2177,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2089,7 +2197,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -2109,7 +2217,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -2129,7 +2237,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2149,7 +2257,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -2169,7 +2277,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2189,7 +2297,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2209,7 +2317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -2229,7 +2337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -2249,7 +2357,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2269,7 +2377,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2303,9 +2411,9 @@
       <selection sqref="A1:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2322,7 +2430,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>180</v>
       </c>
@@ -2353,9 +2461,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2372,7 +2480,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>50</v>
       </c>
@@ -2402,9 +2510,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -2421,7 +2529,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -2441,7 +2549,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2461,7 +2569,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2481,7 +2589,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2501,7 +2609,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>13</v>
       </c>

</xml_diff>